<commit_message>
Class Processor is working. First version of Hierarchy too.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/02_declare_hierarchies_and_cloning_and_scaling.xlsx
+++ b/backend_tests/z_input_files/v2/02_declare_hierarchies_and_cloning_and_scaling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="93">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -138,7 +138,7 @@
     <t xml:space="preserve">Flow</t>
   </si>
   <si>
-    <t xml:space="preserve">Kg</t>
+    <t xml:space="preserve">kg</t>
   </si>
   <si>
     <t xml:space="preserve">Cantaloupe</t>
@@ -219,42 +219,42 @@
     <t xml:space="preserve">Alias</t>
   </si>
   <si>
+    <t xml:space="preserve">WindTurbine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Archetype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nacelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orientation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OppositeProcessorType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">InterfaceAttributes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Location</t>
   </si>
   <si>
-    <t xml:space="preserve">WindTurbine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structural</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Archetype</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nacelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interface</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Orientation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OppositeProcessorType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">InterfaceAttributes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Value</t>
   </si>
   <si>
@@ -282,9 +282,6 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">kg</t>
-  </si>
-  <si>
     <t xml:space="preserve">NominalPower [MW]</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
   </si>
   <si>
     <t xml:space="preserve">Instance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A wind farm</t>
   </si>
   <si>
     <t xml:space="preserve">WindTurbine1</t>
@@ -429,12 +423,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -446,7 +440,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -459,7 +453,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.01"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.91"/>
@@ -615,8 +609,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -629,7 +623,7 @@
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -937,8 +931,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -948,10 +942,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -967,9 +961,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,113 +1000,109 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1160,7 +1149,7 @@
         <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>28</v>
@@ -1175,16 +1164,16 @@
         <v>30</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>76</v>
@@ -1227,7 +1216,7 @@
         <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
@@ -1256,7 +1245,7 @@
         <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
@@ -1270,24 +1259,24 @@
         <v>10000</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R3" s="4" t="n">
         <v>2016</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T3" s="4"/>
       <c r="U3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1295,7 +1284,7 @@
         <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>52</v>
@@ -1304,10 +1293,10 @@
         <v>100</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1315,8 +1304,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1326,10 +1315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1345,9 +1334,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,91 +1373,81 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="4" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1477,8 +1455,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1525,7 +1503,7 @@
         <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>28</v>
@@ -1540,16 +1518,16 @@
         <v>30</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>76</v>
@@ -1592,7 +1570,7 @@
         <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1625,7 +1603,7 @@
         <v>51</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1656,8 +1634,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hierarchy objects are filtered (only Taxon are shown) and sorted (Code list are shown first)
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/02_declare_hierarchies_and_cloning_and_scaling.xlsx
+++ b/backend_tests/z_input_files/v2/02_declare_hierarchies_and_cloning_and_scaling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="96">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t xml:space="preserve">Code 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rafa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HG1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ejemplo</t>
   </si>
   <si>
     <t xml:space="preserve">InterfaceTypeHierarchy</t>
@@ -438,10 +447,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ7"/>
+  <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -604,6 +613,80 @@
         <v>26</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -623,7 +706,7 @@
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -642,19 +725,19 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>9</v>
@@ -663,7 +746,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>10</v>
@@ -672,258 +755,258 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="D3" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F4" s="5"/>
       <c r="H4" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -967,34 +1050,34 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
@@ -1008,19 +1091,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1029,21 +1112,21 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -1052,21 +1135,21 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1075,21 +1158,21 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -1146,81 +1229,81 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1242,14 +1325,14 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -1259,44 +1342,44 @@
         <v>10000</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="R3" s="4" t="n">
         <v>2016</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="T3" s="4"/>
       <c r="U3" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K4" s="1" t="n">
         <v>100</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1317,7 +1400,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -1340,34 +1423,34 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
@@ -1380,19 +1463,19 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1401,53 +1484,53 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1500,77 +1583,77 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1582,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
@@ -1600,10 +1683,10 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1615,7 +1698,7 @@
         <v>4</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>

</xml_diff>

<commit_message>
First version of the flow graph solver working, plus associated changes. Tested.
</commit_message>
<xml_diff>
--- a/backend_tests/z_input_files/v2/02_declare_hierarchies_and_cloning_and_scaling.xlsx
+++ b/backend_tests/z_input_files/v2/02_declare_hierarchies_and_cloning_and_scaling.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hierarchies" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="97">
   <si>
     <t xml:space="preserve">Source</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input</t>
   </si>
   <si>
     <t xml:space="preserve">NominalPower [MW]</t>
@@ -449,8 +452,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1197,8 +1200,8 @@
   </sheetPr>
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T3" activeCellId="0" sqref="T3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S5" activeCellId="0" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1212,7 +1215,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.16"/>
@@ -1309,7 +1312,9 @@
       <c r="F2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1339,7 +1344,9 @@
       <c r="F3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
@@ -1355,7 +1362,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="S3" s="4" t="n">
         <v>2016</v>
@@ -1363,7 +1370,7 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1376,6 +1383,9 @@
       <c r="F4" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="L4" s="1" t="n">
         <v>100</v>
       </c>
@@ -1383,7 +1393,10 @@
         <v>40</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="S4" s="1" t="n">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>
@@ -1467,7 +1480,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1479,7 +1492,7 @@
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -1488,10 +1501,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>68</v>
@@ -1500,15 +1513,15 @@
         <v>69</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>68</v>
@@ -1517,15 +1530,15 @@
         <v>69</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>68</v>
@@ -1534,7 +1547,7 @@
         <v>69</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1555,8 +1568,8 @@
   </sheetPr>
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1570,7 +1583,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="5.16"/>
@@ -1661,11 +1674,13 @@
         <v>54</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1695,11 +1710,13 @@
         <v>54</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>

</xml_diff>